<commit_message>
Rain gauge BOM update
</commit_message>
<xml_diff>
--- a/hardware/Rain Gauge/BOM/BOM.xlsx
+++ b/hardware/Rain Gauge/BOM/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Desktop\Uni\5th year\Semester 2\Project\GitHub Folder\WeirWeather-AWS\hardware\Rain Gauge\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C39CFA4-310E-4B3A-9C4B-FAB4AAD6CE6D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{993B2CD5-33D3-4F84-9F18-784C3960287F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21375" yWindow="3105" windowWidth="14400" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BillOfMaterials" sheetId="2" r:id="rId1"/>
@@ -309,9 +309,6 @@
     <t>Ball bearing</t>
   </si>
   <si>
-    <t>PETG material</t>
-  </si>
-  <si>
     <t>Stainless steel M4 nut</t>
   </si>
   <si>
@@ -346,6 +343,9 @@
   </si>
   <si>
     <t>Total Cost : £ 57.84</t>
+  </si>
+  <si>
+    <t>PETG [Kg]</t>
   </si>
 </sst>
 </file>
@@ -3623,8 +3623,8 @@
   </sheetPr>
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="150" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -3716,7 +3716,7 @@
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="37" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -3728,7 +3728,7 @@
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="41" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -3902,7 +3902,7 @@
         <v>6</v>
       </c>
       <c r="B16" s="62" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C16" s="17"/>
       <c r="D16" s="56">
@@ -3926,7 +3926,7 @@
         <v>7</v>
       </c>
       <c r="B17" s="62" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C17" s="17"/>
       <c r="D17" s="56">
@@ -3998,7 +3998,7 @@
         <v>10</v>
       </c>
       <c r="B20" s="62" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C20" s="17"/>
       <c r="D20" s="56">
@@ -4022,7 +4022,7 @@
         <v>11</v>
       </c>
       <c r="B21" s="62" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="C21" s="17"/>
       <c r="D21" s="56">
@@ -4047,7 +4047,7 @@
         <v>12</v>
       </c>
       <c r="B22" s="62" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C22" s="17"/>
       <c r="D22" s="56">
@@ -4072,7 +4072,7 @@
         <v>13</v>
       </c>
       <c r="B23" s="62" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C23" s="17"/>
       <c r="D23" s="56">
@@ -4097,7 +4097,7 @@
         <v>14</v>
       </c>
       <c r="B24" s="62" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C24" s="17"/>
       <c r="D24" s="56">
@@ -4122,7 +4122,7 @@
         <v>15</v>
       </c>
       <c r="B25" s="62" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C25" s="17"/>
       <c r="D25" s="56">
@@ -4146,7 +4146,7 @@
         <v>14</v>
       </c>
       <c r="B26" s="62" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C26" s="17"/>
       <c r="D26" s="56">
@@ -4170,7 +4170,7 @@
         <v>15</v>
       </c>
       <c r="B27" s="62" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C27" s="17"/>
       <c r="D27" s="56">
@@ -4194,7 +4194,7 @@
         <v>16</v>
       </c>
       <c r="B28" s="63" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C28" s="17"/>
       <c r="D28" s="56">

</xml_diff>